<commit_message>
added testing mode to ensure mails go to certain mail. Added logic for renaming other resumes than mine. LLM response to 20 words.
</commit_message>
<xml_diff>
--- a/contacts/contacts-sample.xlsx
+++ b/contacts/contacts-sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://my.wal-mart.com/personal/s0g0e60_homeoffice_wal-mart_com/Documents/stdy/Auto-emails/contacts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="11_085DF4C7127B1E8F6546807746245E3FB48F8C43" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27474478-65B7-43B5-86B1-79823FC7A1D3}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_085D4FAF146DE26EE742247451245E3FB48F8C25" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2590D93E-50D1-4E35-BA2A-246A36D2D759}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,6 +40,15 @@
     <t>Sent_Indicator</t>
   </si>
   <si>
+    <t>Sample Sample</t>
+  </si>
+  <si>
+    <t>Sample Company</t>
+  </si>
+  <si>
+    <t>domain</t>
+  </si>
+  <si>
     <t>ai</t>
   </si>
   <si>
@@ -47,15 +56,6 @@
   </si>
   <si>
     <t>Molly Cars</t>
-  </si>
-  <si>
-    <t>Sample Sample</t>
-  </si>
-  <si>
-    <t>Sample Company</t>
-  </si>
-  <si>
-    <t>domain</t>
   </si>
   <si>
     <t>No</t>
@@ -424,16 +424,10 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="19.88671875" customWidth="1"/>
-    <col min="2" max="2" width="28.109375" customWidth="1"/>
-    <col min="3" max="3" width="23.21875" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -457,16 +451,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
@@ -474,10 +468,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>

</xml_diff>